<commit_message>
Relationship between lit_mantle compositions with Mg number
</commit_message>
<xml_diff>
--- a/Composition.xlsx
+++ b/Composition.xlsx
@@ -250,11 +250,11 @@
   </sheetPr>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.88"/>

</xml_diff>